<commit_message>
create gerber files, update BOM for REV2
</commit_message>
<xml_diff>
--- a/distortion/BOM.xlsx
+++ b/distortion/BOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/Projekte/Audio/effect-pedals/distortion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11129AA-6FE3-F742-A08B-482E4B27E3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BC1AAB-0CC1-AF44-AA4A-28E02B94994B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{8B7FEFBE-3B34-DE4E-B0EA-C9CB79D86C09}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="rev2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="108">
   <si>
     <t>Designator</t>
   </si>
@@ -74,9 +74,6 @@
     <t>R8</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>R10</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>C8</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>C10</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>CF1</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -263,24 +254,12 @@
     <t>100k</t>
   </si>
   <si>
-    <t>CD1</t>
-  </si>
-  <si>
-    <t>320nF</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
-    <t>3.3k</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
-    <t>20nF</t>
-  </si>
-  <si>
     <t>2k</t>
   </si>
   <si>
@@ -314,18 +293,6 @@
     <t>Fuzz - Model/Value</t>
   </si>
   <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>Foot Switch</t>
-  </si>
-  <si>
-    <t>Audio Jack</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>R_0805-2012</t>
   </si>
   <si>
@@ -333,6 +300,66 @@
   </si>
   <si>
     <t>300Ω</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>PinHeader_1x2</t>
+  </si>
+  <si>
+    <t>9V Barrel Jack</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>RD3</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C_1206-3216</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>PinHeader_1x3</t>
+  </si>
+  <si>
+    <t>PinHeader_2x3</t>
+  </si>
+  <si>
+    <t>39nF</t>
+  </si>
+  <si>
+    <t>510k</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>Rcc3</t>
+  </si>
+  <si>
+    <t>Rcc4</t>
   </si>
 </sst>
 </file>
@@ -444,15 +471,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -774,20 +799,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4154E7-176D-454B-AB9E-4A11C6287C8C}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <pane xSplit="46360" ySplit="1700" topLeftCell="F11" activePane="bottomLeft"/>
+      <pane xSplit="46360" ySplit="1700" topLeftCell="F1" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
       <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" style="2" customWidth="1"/>
   </cols>
@@ -796,205 +821,205 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>34</v>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="10" t="str">
+      <c r="B2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8" t="str">
         <f>C2</f>
         <v>LMR62014XMF-NOPB</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="11" t="str">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="9" t="str">
         <f>C3</f>
         <v>TL081H</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="11" t="str">
-        <f t="shared" ref="D4:D23" si="0">C4</f>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f t="shared" ref="D4:D29" si="0">C4</f>
         <v>TL081H</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>TL081H</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>TLV767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>TL081H</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>TL081H</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>TLV767</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>1N4148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>1N4148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11" t="str">
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>1N4148</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="11" t="str">
+      <c r="B11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>1N4148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>1N4148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>1N4148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>SD0805S020S1R0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Red LED</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>SD0805S020S1R0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>94</v>
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>6.3mm Audio Jack</v>
+        <v>Red LED</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>94</v>
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1003,242 +1028,248 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>USB4125-GF-A-0190</v>
+        <v>6.3mm Audio Jack</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>68</v>
+        <v>46</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>USB4125-GF-A-0190</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>6P DPDT Foot Switch</v>
+        <v>9V Barrel Jack</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>89</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10uH</v>
+        <v>0Ω</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>90</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5.1k</v>
+        <v>0Ω</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>5.1k</v>
+        <v>36</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>45</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10k</v>
+        <v>6P DPDT Foot Switch</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10k</v>
+        <v>10uH</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>48</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10k</v>
+        <v>5.1k</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>96</v>
+        <v>47</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1k</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1k</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>96</v>
+        <v>107</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1k</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>96</v>
+        <v>49</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10k</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>69</v>
+        <v>50</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10k</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>96</v>
+        <v>51</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10k</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>96</v>
+        <v>4</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>96</v>
+        <v>5</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>74</v>
@@ -1249,234 +1280,234 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>96</v>
+        <v>6</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>96</v>
+        <v>7</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>96</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>96</v>
+        <v>12</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>97</v>
+        <v>13</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>97</v>
+        <v>14</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>97</v>
+        <v>15</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>97</v>
+        <v>17</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>97</v>
+        <v>18</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>97</v>
+        <v>19</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>80</v>
@@ -1487,100 +1518,212 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>97</v>
+        <v>20</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>97</v>
+        <v>21</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>97</v>
+        <v>22</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>97</v>
+        <v>24</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>97</v>
+        <v>25</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>75</v>
-      </c>
-      <c r="B55" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>68</v>
+      <c r="B62" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>